<commit_message>
Edited the xlsx file for test purpose
</commit_message>
<xml_diff>
--- a/resources/testdata/LoginTestCases.xlsx
+++ b/resources/testdata/LoginTestCases.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
-    <sheet name="Test_A" sheetId="2" r:id="rId2"/>
+    <sheet name="verifyISPUserSuccessfulLogin" sheetId="2" r:id="rId2"/>
     <sheet name="Test_C" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>TCID</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Subject</t>
-  </si>
-  <si>
     <t>Pratap</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>csm10002</t>
   </si>
   <si>
-    <t>Eng</t>
-  </si>
-  <si>
     <t>Error</t>
   </si>
   <si>
@@ -75,9 +69,6 @@
     <t>csm10003</t>
   </si>
   <si>
-    <t>Bng</t>
-  </si>
-  <si>
     <t>Roll_NO</t>
   </si>
   <si>
@@ -88,6 +79,21 @@
   </si>
   <si>
     <t>verifyNoCredentialAtLoginError</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Div</t>
+  </si>
+  <si>
+    <t>!st</t>
+  </si>
+  <si>
+    <t>fadmin</t>
+  </si>
+  <si>
+    <t>2nd</t>
   </si>
 </sst>
 </file>
@@ -438,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +468,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -473,7 +479,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -484,7 +490,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -500,15 +506,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -516,70 +522,29 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
+      <c r="C3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +567,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>10</v>
@@ -611,18 +576,18 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>12</v>
@@ -633,10 +598,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>22</v>
@@ -647,10 +612,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>12</v>

</xml_diff>

<commit_message>
Adding org related tests
</commit_message>
<xml_diff>
--- a/resources/testdata/LoginTestCases.xlsx
+++ b/resources/testdata/LoginTestCases.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
-    <sheet name="ISPUserSuccessfulLogin" sheetId="2" r:id="rId2"/>
-    <sheet name="ISPLoginWithInvalidPswd" sheetId="3" r:id="rId3"/>
+    <sheet name="resellerUserSuccessfulLogin" sheetId="6" r:id="rId2"/>
+    <sheet name="AgentUserSuccessfulLogin" sheetId="5" r:id="rId3"/>
+    <sheet name="OrgUserSuccessfulLogin" sheetId="4" r:id="rId4"/>
+    <sheet name="ISPUserSuccessfulLogin" sheetId="2" r:id="rId5"/>
+    <sheet name="ISPLoginWithInvalidPswd" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>TCID</t>
   </si>
@@ -61,16 +64,51 @@
   </si>
   <si>
     <t>NoCredentialAtLogin</t>
+  </si>
+  <si>
+    <t>OrgUserSuccessfulLogin</t>
+  </si>
+  <si>
+    <t>autotestuser1@10000.escm.local</t>
+  </si>
+  <si>
+    <t>AgentUserSuccessfulLogin</t>
+  </si>
+  <si>
+    <t>autotestagentuser1@10000_par.escm.local</t>
+  </si>
+  <si>
+    <t>Independent12#</t>
+  </si>
+  <si>
+    <t>resellerUserSuccessfulLogin</t>
+  </si>
+  <si>
+    <t>autotestreseller1@10003_res.escm.local</t>
+  </si>
+  <si>
+    <t>NoPasswordAtLogin</t>
+  </si>
+  <si>
+    <t>NoUserNameAtLogin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,15 +143,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -416,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F10:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,6 +514,46 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -482,8 +563,113 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>